<commit_message>
feat: Update project journal with latest entries and modifications
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_DaSilvaJussani_Joao_Victor_pt2.xlsx
+++ b/Docs/Journal-de-Travail_DaSilvaJussani_Joao_Victor_pt2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg05lby\Documents\GitHub\Flashcards\Flashcards\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg05lby\Documents\GitHub\Flashcards\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDAEC94-18D2-43C8-B9E0-EB442B994D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889AC181-B56E-45F9-81C6-438C2436DE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="31695" yWindow="2625" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Auteur:</t>
   </si>
@@ -158,6 +158,57 @@
   </si>
   <si>
     <t>dockerisation, 100% erreur, je suis toujours au point de départ pour cela</t>
+  </si>
+  <si>
+    <t>Dockerisation complète et fonctionnelle</t>
+  </si>
+  <si>
+    <t>Aidée par Eithan et Théo</t>
+  </si>
+  <si>
+    <t>Modification de la partie "exercer"</t>
+  </si>
+  <si>
+    <t>Ajout du mode jusqu'au bout</t>
+  </si>
+  <si>
+    <t>Ajout d'un bouton d'abandon dans le mode jusqu'au bout</t>
+  </si>
+  <si>
+    <t>Pouvoir choisir si on veut faire question à réponse ou réponse à question</t>
+  </si>
+  <si>
+    <t>mettre une limite de 10 decks et après devoir changer de page "page 2"</t>
+  </si>
+  <si>
+    <t>Avoir un QRCode généré pour pouvoir partagé les decks publics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer la barre de navigation + logo </t>
+  </si>
+  <si>
+    <t>Des messages de validation dans la page register</t>
+  </si>
+  <si>
+    <t>Ajout de la page de profile et de la visite de la page de profile des autres utilisateurs</t>
+  </si>
+  <si>
+    <t>Quand cliquer sur l'auteur du deck public, on peut voir sa page de profile</t>
+  </si>
+  <si>
+    <t>Créer un composant pour les header</t>
+  </si>
+  <si>
+    <t>Ajout d'un bouton d'aide pour les utilisateurs</t>
+  </si>
+  <si>
+    <t>Un système de followers</t>
+  </si>
+  <si>
+    <t>Barre de recherche dynamique</t>
+  </si>
+  <si>
+    <t>pouvoir afficher en liste ou en grid</t>
   </si>
 </sst>
 </file>
@@ -425,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -615,6 +666,10 @@
     <xf numFmtId="10" fontId="11" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -625,8 +680,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -634,6 +689,90 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -809,90 +948,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1174,7 +1229,7 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405</c:v>
+                  <c:v>1530</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>225</c:v>
@@ -2104,13 +2159,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6.6666666666666666E-2</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4095,18 +4150,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="15">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4301,8 +4356,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4334,15 +4389,15 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="84" t="s">
+      <c r="B2" s="87"/>
+      <c r="C2" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -4351,13 +4406,13 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>11 heures 15 minutes</v>
+        <v>30 heures 0 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4372,24 +4427,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>420</v>
+        <v>1140</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>255</v>
+        <v>660</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>675</v>
+        <v>1800</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="85"/>
+      <c r="D5" s="86"/>
     </row>
     <row r="6" spans="1:15" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
@@ -4478,7 +4533,7 @@
       <c r="E9" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="84" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="40"/>
@@ -4608,16 +4663,28 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="str">
+      <c r="A14" s="62">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="39"/>
+        <v>18</v>
+      </c>
+      <c r="B14" s="30">
+        <v>45777</v>
+      </c>
+      <c r="C14" s="31">
+        <v>3</v>
+      </c>
+      <c r="D14" s="32">
+        <v>45</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>40</v>
+      </c>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4626,15 +4693,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="63" t="str">
+      <c r="A15" s="63">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="23"/>
+        <v>19</v>
+      </c>
+      <c r="B15" s="34">
+        <v>45784</v>
+      </c>
+      <c r="C15" s="35">
+        <v>2</v>
+      </c>
+      <c r="D15" s="36">
+        <v>0</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>41</v>
+      </c>
       <c r="G15" s="40"/>
       <c r="N15">
         <v>8</v>
@@ -4649,25 +4726,41 @@
         <v/>
       </c>
       <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="23"/>
+      <c r="C16" s="31">
+        <v>1</v>
+      </c>
+      <c r="D16" s="32">
+        <v>45</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="39"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="str">
+      <c r="A17" s="63">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="B17" s="34">
+        <v>45791</v>
+      </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="23"/>
+      <c r="D17" s="32">
+        <v>30</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G17" s="40"/>
       <c r="O17">
         <v>45</v>
@@ -4679,10 +4772,18 @@
         <v/>
       </c>
       <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="23"/>
+      <c r="C18" s="31">
+        <v>1</v>
+      </c>
+      <c r="D18" s="88">
+        <v>0</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="G18" s="39"/>
       <c r="O18">
         <v>50</v>
@@ -4695,9 +4796,15 @@
       </c>
       <c r="B19" s="34"/>
       <c r="C19" s="35"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="36">
+        <v>30</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="G19" s="40"/>
       <c r="O19">
         <v>55</v>
@@ -4709,10 +4816,18 @@
         <v/>
       </c>
       <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="23"/>
+      <c r="C20" s="31">
+        <v>1</v>
+      </c>
+      <c r="D20" s="32">
+        <v>30</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -4722,21 +4837,37 @@
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="23"/>
+      <c r="D21" s="36">
+        <v>15</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="23"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45798</v>
+      </c>
+      <c r="C22" s="31">
+        <v>1</v>
+      </c>
+      <c r="D22" s="32">
+        <v>0</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>48</v>
+      </c>
       <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -4745,10 +4876,18 @@
         <v/>
       </c>
       <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="23"/>
+      <c r="C23" s="35">
+        <v>1</v>
+      </c>
+      <c r="D23" s="36">
+        <v>30</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -4757,22 +4896,38 @@
         <v/>
       </c>
       <c r="B24" s="30"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="23"/>
+      <c r="C24" s="31">
+        <v>1</v>
+      </c>
+      <c r="D24" s="32">
+        <v>15</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="str">
+      <c r="A25" s="63">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="34"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="34">
+        <v>45805</v>
+      </c>
       <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="23"/>
+      <c r="D25" s="36">
+        <v>30</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -4782,9 +4937,15 @@
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="23"/>
+      <c r="D26" s="32">
+        <v>30</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>52</v>
+      </c>
       <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -4793,10 +4954,18 @@
         <v/>
       </c>
       <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="23"/>
+      <c r="C27" s="35">
+        <v>1</v>
+      </c>
+      <c r="D27" s="36">
+        <v>30</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -4806,9 +4975,15 @@
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="22"/>
+      <c r="D28" s="32">
+        <v>30</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -4818,9 +4993,15 @@
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="22"/>
+      <c r="D29" s="36">
+        <v>45</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -10868,31 +11049,31 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$E7="Absent"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="10" stopIfTrue="1">
       <formula>$E7="Implémentation"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10900,11 +11081,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C532" xr:uid="{9D52E29F-610D-40B2-B3CC-F94A741DD978}">
       <formula1>$N$7:$N$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D532" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
-      <formula1>$O$7:$O$19</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E532" xr:uid="{EBCA439E-C5F1-BC4C-88EE-2BB045537E3E}">
       <formula1>$M$7:$M$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19:D532 D7:D17" xr:uid="{46510F84-8BCC-4BD6-9A19-9F03ACD74D05}">
+      <formula1>$O$7:$O$19</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11018,7 +11199,7 @@
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>6.6666666666666666E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11035,15 +11216,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>960</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>165</v>
+        <v>570</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>405</v>
+        <v>1530</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11051,11 +11232,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>6 h 45 min</v>
+        <v>25 h 30 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.6</v>
+        <v>0.85</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11092,7 +11273,7 @@
       </c>
       <c r="G8" s="72">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="L8" s="54" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11181,26 +11362,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>420</v>
+        <v>1140</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>255</v>
+        <v>660</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>675</v>
+        <v>1800</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>11 h 15 min</v>
+        <v>30 h 00 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>0.12784090909090909</v>
+        <v>0.34090909090909088</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11244,26 +11425,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11464,10 +11625,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11486,20 +11678,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>